<commit_message>
Update market data, stock prices, and stock files
🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/dumps/Stocks/Adani Power Limited.xlsx
+++ b/dumps/Stocks/Adani Power Limited.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB5"/>
+  <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -574,36 +574,105 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>40</v>
+      </c>
+      <c r="E5" t="n">
+        <v>152.24</v>
+      </c>
+      <c r="F5" t="n">
+        <v>6120</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>CN#252611665409</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>30.4</v>
+      </c>
+      <c r="J5">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>46062</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>40</v>
+      </c>
+      <c r="E6" t="n">
+        <v>149.76</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5990.4</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>~</t>
+        </is>
+      </c>
+      <c r="J6">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
         <v>46063</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>NSE</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="D7" t="n">
         <v>20</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E7" t="n">
         <v>148.71</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F7" t="n">
         <v>2989</v>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>CN#252611730667</t>
         </is>
       </c>
-      <c r="I5" t="n">
+      <c r="I7" t="n">
         <v>14.8</v>
       </c>
-      <c r="J5">
+      <c r="J7">
         <f>Index!$C$2</f>
         <v/>
       </c>

</xml_diff>